<commit_message>
Finished the Web GUI phptravels assignment tests
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AdminUserTestData.xlsx
+++ b/src/test/resources/TestData/AdminUserTestData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.elsharkawy\git\Automation-Assignment\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D6E1BC-20D7-4EE9-BBCF-D5A0B7B55975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14232" windowHeight="3264"/>
   </bookViews>
   <sheets>
     <sheet name="adminUser" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>FirstName</t>
   </si>
@@ -51,34 +50,55 @@
     <t>m1155150745</t>
   </si>
   <si>
-    <t>TC ID/Name</t>
-  </si>
-  <si>
-    <t>testingValidUserSignUp</t>
-  </si>
-  <si>
-    <t>Mobile Number</t>
-  </si>
-  <si>
-    <t>testingInvalidUserSignUp_emailAlreadyExists</t>
-  </si>
-  <si>
-    <t>testingInvalidUserSignUp_emailWrongFormat</t>
-  </si>
-  <si>
-    <t>Expected Alert Message</t>
-  </si>
-  <si>
-    <t>Email Already Exists.</t>
-  </si>
-  <si>
-    <t>The Email field must contain a valid email address.</t>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>adress1</t>
+  </si>
+  <si>
+    <t>adress2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>EmailDomain</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>NewCity</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -129,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -140,6 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,114 +474,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A63622E-CB57-6443-8D5E-E59E3D20E8B5}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4">
+        <v>12345678901</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1155150745</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1155150745</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1155150745</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>